<commit_message>
fixes for excel download
</commit_message>
<xml_diff>
--- a/Backend/store/output.xlsx
+++ b/Backend/store/output.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -31,40 +31,16 @@
     <t>AMOUNT</t>
   </si>
   <si>
-    <t>2023-04-14T14:55</t>
-  </si>
-  <si>
-    <t>Santosh Yadav</t>
+    <t>2023-04-17T12:34</t>
+  </si>
+  <si>
+    <t>Master</t>
   </si>
   <si>
     <t>Cash</t>
   </si>
   <si>
-    <t>Advance for t site</t>
-  </si>
-  <si>
-    <t>2023-04-14T15:29</t>
-  </si>
-  <si>
-    <t>Advance from Santosh for furniture work.</t>
-  </si>
-  <si>
-    <t>2023-04-15T15:30</t>
-  </si>
-  <si>
-    <t>Credit-Card</t>
-  </si>
-  <si>
-    <t>Remaining payment for the site.</t>
-  </si>
-  <si>
-    <t>2023-04-22T15:47</t>
-  </si>
-  <si>
-    <t>Amazon-Pay</t>
-  </si>
-  <si>
-    <t>Advance from Santosh yadav for furniture and pop contract</t>
+    <t>advance</t>
   </si>
 </sst>
 </file>
@@ -456,7 +432,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
@@ -503,67 +479,7 @@
         <v>9</v>
       </c>
       <c r="F2" s="3">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="3">
-        <v>25000.65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="3">
-        <v>460000.54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="3">
-        <v>56000</v>
+        <v>44999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Latest changes - 14:48-17-april-23
</commit_message>
<xml_diff>
--- a/Backend/store/output.xlsx
+++ b/Backend/store/output.xlsx
@@ -31,7 +31,7 @@
     <t>AMOUNT</t>
   </si>
   <si>
-    <t>2023-04-17T12:34</t>
+    <t>12/04/23</t>
   </si>
   <si>
     <t>Master</t>
@@ -40,7 +40,7 @@
     <t>Cash</t>
   </si>
   <si>
-    <t>advance</t>
+    <t>etygf</t>
   </si>
 </sst>
 </file>
@@ -479,7 +479,7 @@
         <v>9</v>
       </c>
       <c r="F2" s="3">
-        <v>44999</v>
+        <v>4522</v>
       </c>
     </row>
   </sheetData>

</xml_diff>